<commit_message>
- ‘BH/DESCRIPTION’ - ‘BH/INDEX’ - ‘BH/MD5’ - ‘BH/Meta/Rd.rds’ - ‘BH/Meta/hsearch.rds’ - ‘BH/Meta/links.rds’ - ‘BH/Meta/nsInfo.rds’ - ‘BH/Meta/package.rds’ - ‘BH/NAMESPACE’ - ‘BH/NEWS.Rd’ ...
</commit_message>
<xml_diff>
--- a/gdata/xls/ExampleExcelFile.xlsx
+++ b/gdata/xls/ExampleExcelFile.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="23980" windowHeight="17340" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14780" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet First" sheetId="1" r:id="rId1"/>
@@ -12,9 +12,9 @@
     <sheet name="Sheet with a very long name!" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet with initial text" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -127,8 +127,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss.00"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -152,6 +155,18 @@
       <i/>
       <sz val="10"/>
       <color indexed="57"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Verdana"/>
     </font>
   </fonts>
@@ -179,24 +194,28 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -213,80 +232,18 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00DD0806"/>
-      <rgbColor rgb="001FB714"/>
-      <rgbColor rgb="000000D4"/>
-      <rgbColor rgb="00FCF305"/>
-      <rgbColor rgb="00F20884"/>
-      <rgbColor rgb="0000ABEA"/>
-      <rgbColor rgb="00900000"/>
-      <rgbColor rgb="00006411"/>
-      <rgbColor rgb="00000090"/>
-      <rgbColor rgb="0090713A"/>
-      <rgbColor rgb="004600A5"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="0063AAFE"/>
-      <rgbColor rgb="00DD2D32"/>
-      <rgbColor rgb="00FFF58C"/>
-      <rgbColor rgb="004EE257"/>
-      <rgbColor rgb="006711FF"/>
-      <rgbColor rgb="00FEA746"/>
-      <rgbColor rgb="00865357"/>
-      <rgbColor rgb="00A2BD90"/>
-      <rgbColor rgb="0063AAFE"/>
-      <rgbColor rgb="00DD2D32"/>
-      <rgbColor rgb="00FFF58C"/>
-      <rgbColor rgb="004EE257"/>
-      <rgbColor rgb="006711FF"/>
-      <rgbColor rgb="00FEA746"/>
-      <rgbColor rgb="00865357"/>
-      <rgbColor rgb="00A2BD90"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -609,14 +566,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
@@ -731,7 +688,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -739,14 +696,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
@@ -853,12 +810,11 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -866,21 +822,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="7" max="7" width="19.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" s="7">
-        <v>35430</v>
+        <v>36892</v>
       </c>
       <c r="C1" s="8">
         <v>4.2361111111111106E-2</v>
@@ -896,13 +856,20 @@
       <c r="F1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="10">
+        <v>36892.042372800926</v>
+      </c>
+      <c r="H1" s="11">
+        <f>G1</f>
+        <v>36892.042372800926</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2" s="7">
-        <v>35827</v>
+        <v>37289</v>
       </c>
       <c r="C2" s="8">
         <v>8.4722222222222213E-2</v>
@@ -918,13 +885,20 @@
       <c r="F2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="10">
+        <v>37289.084745601853</v>
+      </c>
+      <c r="H2" s="11">
+        <f t="shared" ref="H2:H10" si="1">G2</f>
+        <v>37289.084745601853</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3" s="7">
-        <v>36221</v>
+        <v>37683</v>
       </c>
       <c r="C3" s="8">
         <v>0.12708333333333333</v>
@@ -940,13 +914,20 @@
       <c r="F3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="10">
+        <v>37683.127118402779</v>
+      </c>
+      <c r="H3" s="11">
+        <f t="shared" si="1"/>
+        <v>37683.127118402779</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" s="7">
-        <v>36619</v>
+        <v>38081</v>
       </c>
       <c r="C4" s="8">
         <v>0.16944444444444443</v>
@@ -959,13 +940,20 @@
         <f>E3^2</f>
         <v>0.70807341827357118</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="10">
+        <v>38081.169491203706</v>
+      </c>
+      <c r="H4" s="11">
+        <f t="shared" si="1"/>
+        <v>38081.169491203706</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5" s="7">
-        <v>37015</v>
+        <v>38477</v>
       </c>
       <c r="C5" s="8">
         <v>0.21180555555555555</v>
@@ -975,19 +963,26 @@
         <v>0.46022337571613586</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:E10" si="1">E4^2</f>
+        <f t="shared" ref="E5:E10" si="2">E4^2</f>
         <v>0.5013679656656197</v>
       </c>
       <c r="F5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="10">
+        <v>38477.211864004632</v>
+      </c>
+      <c r="H5" s="11">
+        <f t="shared" si="1"/>
+        <v>38477.211864004632</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6" s="7">
-        <v>37412</v>
+        <v>38874</v>
       </c>
       <c r="C6" s="8">
         <v>0.25416666666666665</v>
@@ -996,19 +991,26 @@
         <v>22</v>
       </c>
       <c r="E6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.25136983699568199</v>
       </c>
       <c r="F6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="10">
+        <v>38874.254236805558</v>
+      </c>
+      <c r="H6" s="11">
+        <f t="shared" si="1"/>
+        <v>38874.254236805558</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" s="7">
-        <v>37808</v>
+        <v>39270</v>
       </c>
       <c r="C7" s="8">
         <v>0.29652777777777778</v>
@@ -1018,19 +1020,26 @@
         <v>0.54454364175681802</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.3186794951235734E-2</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="10">
+        <v>39270.296609606485</v>
+      </c>
+      <c r="H7" s="11">
+        <f t="shared" si="1"/>
+        <v>39270.296609606485</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" s="7">
-        <v>38206</v>
+        <v>39668</v>
       </c>
       <c r="C8" s="8">
         <v>0.33888888888888885</v>
@@ -1042,13 +1051,20 @@
       <c r="F8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="10">
+        <v>39668.338982407404</v>
+      </c>
+      <c r="H8" s="11">
+        <f t="shared" si="1"/>
+        <v>39668.338982407404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9" s="7">
-        <v>38603</v>
+        <v>40065</v>
       </c>
       <c r="C9" s="8">
         <v>0.38125000000000003</v>
@@ -1058,19 +1074,26 @@
         <v>0.61745445176142344</v>
       </c>
       <c r="E9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="10">
+        <v>40065.38135520833</v>
+      </c>
+      <c r="H9" s="11">
+        <f t="shared" si="1"/>
+        <v>40065.38135520833</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10" s="7">
-        <v>38999</v>
+        <v>40461</v>
       </c>
       <c r="C10" s="8">
         <v>0.4236111111111111</v>
@@ -1080,20 +1103,26 @@
         <v>0.65085413965888783</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F10" t="s">
         <v>18</v>
       </c>
+      <c r="G10" s="10">
+        <v>40461.423728009257</v>
+      </c>
+      <c r="H10" s="11">
+        <f t="shared" si="1"/>
+        <v>40461.423728009257</v>
+      </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -1101,14 +1130,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -1218,12 +1247,11 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>